<commit_message>
Fix: Wrong negative times
</commit_message>
<xml_diff>
--- a/timesheet-template.xlsx
+++ b/timesheet-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="دورکاری" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">دورکاری!$A$1:$W$39</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">دورکاری!$A$1:$W$39</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">دورکاری!$A$1:$W$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">دورکاری!$A$1:$W$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -850,48 +851,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>-255240</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>-159480</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="-2084040" y="38160"/>
-          <a:ext cx="1762920" cy="844560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -899,26 +858,26 @@
   </sheetPr>
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.00892857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.78125"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="8" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="2.00892857142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.4330357142857"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="3.78125"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="2.00892857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.88839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.66071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="8" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="1.88839285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.0803571428571"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="3.66071428571429"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.88839285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="7.20535714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1120,34 +1079,34 @@
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18" t="n">
         <v>0</v>
@@ -1170,34 +1129,34 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="18" t="n">
         <v>0</v>
@@ -1220,34 +1179,34 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8" s="18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N8" s="18" t="n">
         <v>0</v>
@@ -1270,34 +1229,34 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M9" s="18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N9" s="18" t="n">
         <v>0</v>
@@ -1320,34 +1279,34 @@
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M10" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N10" s="18" t="n">
         <v>0</v>
@@ -1370,34 +1329,34 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M11" s="18" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N11" s="18" t="n">
         <v>0</v>
@@ -1420,34 +1379,34 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M12" s="18" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N12" s="18" t="n">
         <v>0</v>
@@ -1470,34 +1429,34 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M13" s="18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N13" s="18" t="n">
         <v>0</v>
@@ -1520,34 +1479,34 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M14" s="18" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="N14" s="18" t="n">
         <v>0</v>
@@ -1570,34 +1529,34 @@
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N15" s="18" t="n">
         <v>0</v>
@@ -1620,34 +1579,34 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M16" s="18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N16" s="18" t="n">
         <v>0</v>
@@ -1670,34 +1629,34 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M17" s="18" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N17" s="18" t="n">
         <v>0</v>
@@ -1720,34 +1679,34 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M18" s="18" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="N18" s="18" t="n">
         <v>0</v>
@@ -1770,34 +1729,34 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M19" s="18" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N19" s="18" t="n">
         <v>0</v>
@@ -1820,34 +1779,34 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="M20" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="N20" s="18" t="n">
         <v>0</v>
@@ -1870,34 +1829,34 @@
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="M21" s="18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N21" s="18" t="n">
         <v>0</v>
@@ -1920,34 +1879,34 @@
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="I22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="L22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M22" s="18" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N22" s="18" t="n">
         <v>0</v>
@@ -1970,34 +1929,34 @@
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M23" s="18" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N23" s="18" t="n">
         <v>0</v>
@@ -2020,34 +1979,34 @@
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="I24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="J24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="K24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="L24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="M24" s="18" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="N24" s="18" t="n">
         <v>0</v>
@@ -2070,34 +2029,34 @@
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M25" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N25" s="18" t="n">
         <v>0</v>
@@ -2120,34 +2079,34 @@
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="L26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="M26" s="18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="N26" s="18" t="n">
         <v>0</v>
@@ -2170,34 +2129,34 @@
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="I27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="K27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="L27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="M27" s="18" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="N27" s="18" t="n">
         <v>0</v>
@@ -2220,34 +2179,34 @@
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="J28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="L28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="M28" s="18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="N28" s="18" t="n">
         <v>0</v>
@@ -2270,34 +2229,34 @@
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="J29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="M29" s="18" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N29" s="18" t="n">
         <v>0</v>
@@ -2320,34 +2279,34 @@
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M30" s="18" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N30" s="18" t="n">
         <v>0</v>
@@ -2370,34 +2329,34 @@
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="G31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="M31" s="18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="N31" s="18" t="n">
         <v>0</v>
@@ -2420,34 +2379,34 @@
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="J32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="K32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="L32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="M32" s="18" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="N32" s="18" t="n">
         <v>0</v>
@@ -2470,34 +2429,34 @@
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="H33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="M33" s="18" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N33" s="18" t="n">
         <v>0</v>
@@ -2520,34 +2479,34 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="F34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="J34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="K34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="L34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="M34" s="18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N34" s="18" t="n">
         <v>0</v>
@@ -2570,34 +2529,34 @@
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M35" s="18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="N35" s="18" t="n">
         <v>0</v>
@@ -2723,6 +2682,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>